<commit_message>
Check of Max, change for rounding
</commit_message>
<xml_diff>
--- a/Assignment 2/EGI_Assignment2_NuurVdVelGrotz.xlsx
+++ b/Assignment 2/EGI_Assignment2_NuurVdVelGrotz.xlsx
@@ -501,7 +501,7 @@
         <v>58.7204</v>
       </c>
       <c r="H3">
-        <v>556.0753999999999</v>
+        <v>556.0754</v>
       </c>
       <c r="I3">
         <v>1.1145</v>
@@ -736,7 +736,7 @@
         <v>73.1567</v>
       </c>
       <c r="H8">
-        <v>877.7012999999999</v>
+        <v>877.7013</v>
       </c>
       <c r="I8">
         <v>1.1613</v>
@@ -745,7 +745,7 @@
         <v>0.06320000000000001</v>
       </c>
       <c r="K8">
-        <v>97.9081</v>
+        <v>97.90810000000001</v>
       </c>
       <c r="L8">
         <v>11.3267</v>
@@ -783,7 +783,7 @@
         <v>76.31140000000001</v>
       </c>
       <c r="H9">
-        <v>950.8579999999999</v>
+        <v>950.858</v>
       </c>
       <c r="I9">
         <v>1.1712</v>
@@ -1400,7 +1400,7 @@
         <v>1.3244</v>
       </c>
       <c r="J22">
-        <v>0.0806</v>
+        <v>0.08060000000000001</v>
       </c>
       <c r="K22">
         <v>167.7695</v>
@@ -2751,7 +2751,7 @@
         <v>0</v>
       </c>
       <c r="F51">
-        <v>516.5078999999999</v>
+        <v>516.5079</v>
       </c>
       <c r="G51">
         <v>361.5555</v>
@@ -3127,7 +3127,7 @@
         <v>0</v>
       </c>
       <c r="F59">
-        <v>678.7412</v>
+        <v>678.7412000000001</v>
       </c>
       <c r="G59">
         <v>475.1188</v>
@@ -3174,7 +3174,7 @@
         <v>0</v>
       </c>
       <c r="F60">
-        <v>702.0676999999999</v>
+        <v>702.0677</v>
       </c>
       <c r="G60">
         <v>491.4474</v>
@@ -3189,7 +3189,7 @@
         <v>0.1916</v>
       </c>
       <c r="K60">
-        <v>567.5827</v>
+        <v>567.5827000000001</v>
       </c>
       <c r="L60">
         <v>30.1</v>
@@ -3221,7 +3221,7 @@
         <v>0</v>
       </c>
       <c r="F61">
-        <v>726.1378999999999</v>
+        <v>726.1379</v>
       </c>
       <c r="G61">
         <v>508.2966</v>
@@ -3365,7 +3365,7 @@
         <v>803.0232</v>
       </c>
       <c r="G64">
-        <v>562.1162</v>
+        <v>562.1162000000001</v>
       </c>
       <c r="H64">
         <v>14494.6271</v>
@@ -3647,7 +3647,7 @@
         <v>979.8393</v>
       </c>
       <c r="G70">
-        <v>685.8875</v>
+        <v>685.8875000000001</v>
       </c>
       <c r="H70">
         <v>18165.7325</v>
@@ -3659,7 +3659,7 @@
         <v>0.2475</v>
       </c>
       <c r="K70">
-        <v>737.3354</v>
+        <v>737.3354000000001</v>
       </c>
       <c r="L70">
         <v>33.6556</v>
@@ -3882,7 +3882,7 @@
         <v>1153.7024</v>
       </c>
       <c r="G75">
-        <v>807.5916999999999</v>
+        <v>807.5917</v>
       </c>
       <c r="H75">
         <v>21831.3385</v>
@@ -3976,7 +3976,7 @@
         <v>1230.7573</v>
       </c>
       <c r="G77">
-        <v>861.5300999999999</v>
+        <v>861.5301</v>
       </c>
       <c r="H77">
         <v>23473.0975</v>
@@ -4223,7 +4223,7 @@
         <v>0.3342</v>
       </c>
       <c r="K82">
-        <v>961.3807</v>
+        <v>961.3807000000001</v>
       </c>
       <c r="L82">
         <v>36.6535</v>
@@ -4495,7 +4495,7 @@
         <v>0.0576</v>
       </c>
       <c r="K5">
-        <v>86.495</v>
+        <v>86.49500000000001</v>
       </c>
       <c r="L5">
         <v>10.467</v>
@@ -4527,7 +4527,7 @@
         <v>0.05</v>
       </c>
       <c r="F6">
-        <v>95.91079999999999</v>
+        <v>95.9108</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -7112,7 +7112,7 @@
         <v>0.05</v>
       </c>
       <c r="F61">
-        <v>756.9115</v>
+        <v>756.9115000000001</v>
       </c>
       <c r="G61">
         <v>0</v>
@@ -8565,7 +8565,7 @@
         <v>52.0494</v>
       </c>
       <c r="H9">
-        <v>813.7012999999999</v>
+        <v>813.7013</v>
       </c>
       <c r="I9">
         <v>1.1524</v>
@@ -9678,7 +9678,7 @@
         <v>12.5769</v>
       </c>
       <c r="C33">
-        <v>787.1461</v>
+        <v>787.1461000000001</v>
       </c>
       <c r="D33">
         <v>13.0125</v>
@@ -11244,7 +11244,7 @@
         <v>286.0613</v>
       </c>
       <c r="H66">
-        <v>8838.4791</v>
+        <v>8838.479100000001</v>
       </c>
       <c r="I66">
         <v>1.9116</v>
@@ -11300,7 +11300,7 @@
         <v>0.1575</v>
       </c>
       <c r="K67">
-        <v>763.8508</v>
+        <v>763.8508000000001</v>
       </c>
       <c r="L67">
         <v>36.4707</v>
@@ -13071,7 +13071,7 @@
         <v>-0.1505</v>
       </c>
       <c r="I32">
-        <v>-9.6225</v>
+        <v>-9.622500000000001</v>
       </c>
       <c r="J32">
         <v>-6.5383</v>
@@ -13251,7 +13251,7 @@
         <v>15.7698</v>
       </c>
       <c r="E38">
-        <v>0.07539999999999999</v>
+        <v>0.0754</v>
       </c>
       <c r="F38">
         <v>-0.3222</v>
@@ -13420,7 +13420,7 @@
         <v>0.127</v>
       </c>
       <c r="H43">
-        <v>-0.06909999999999999</v>
+        <v>-0.0691</v>
       </c>
       <c r="I43">
         <v>-9.326000000000001</v>
@@ -13836,7 +13836,7 @@
         <v>0.4231</v>
       </c>
       <c r="H56">
-        <v>0.06279999999999999</v>
+        <v>0.0628</v>
       </c>
       <c r="I56">
         <v>-5.6528</v>
@@ -14054,7 +14054,7 @@
         <v>3.7498</v>
       </c>
       <c r="F63">
-        <v>0.931</v>
+        <v>0.9310000000000001</v>
       </c>
       <c r="G63">
         <v>0.6015</v>
@@ -14281,7 +14281,7 @@
         <v>1.8805</v>
       </c>
       <c r="G70">
-        <v>0.7909</v>
+        <v>0.7909000000000001</v>
       </c>
       <c r="H70">
         <v>0.2445</v>
@@ -14511,7 +14511,7 @@
         <v>0.3444</v>
       </c>
       <c r="I77">
-        <v>9.2963</v>
+        <v>9.296300000000001</v>
       </c>
       <c r="J77">
         <v>-3.4345</v>

</xml_diff>